<commit_message>
updated labels in results
</commit_message>
<xml_diff>
--- a/documents/Stats_Comparision.xlsx
+++ b/documents/Stats_Comparision.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\Personal\Simulate_Branch_Prediction\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060A69F1-7142-4036-AC1E-79A84DAF9ED8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4438056E-ED69-4108-B8D8-9DF9444FC348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,10 +60,10 @@
     <t xml:space="preserve">Branch </t>
   </si>
   <si>
-    <t>Correct Branch Prediction 2-bit %</t>
+    <t>Incorrect Branch Prediction % 2-bit</t>
   </si>
   <si>
-    <t>Correct Branch Prediction 3-bit %</t>
+    <t>Incorrect Branch Prediction % 3-bit</t>
   </si>
 </sst>
 </file>
@@ -341,7 +341,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="2800"/>
-              <a:t>Comparision of Miss Branch Prediction % </a:t>
+              <a:t>Comparision of Incorrect Branch</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2800" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2800"/>
+              <a:t>Prediction % </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -391,7 +399,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Correct Branch Prediction 2-bit %</c:v>
+                  <c:v>Incorrect Branch Prediction % 2-bit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -548,7 +556,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Correct Branch Prediction 3-bit %</c:v>
+                  <c:v>Incorrect Branch Prediction % 3-bit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -877,7 +885,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="2400"/>
-                  <a:t>Miss Prediction %</a:t>
+                  <a:t>Incorrect</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="2400"/>
+                  <a:t>Prediction %</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1932,8 +1948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>